<commit_message>
Cleanup to readme and template
</commit_message>
<xml_diff>
--- a/python_examples/create_tags/tagging.xlsx
+++ b/python_examples/create_tags/tagging.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dean.kooiman/git/api-examples/python_examples/create_tags/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC27F53-14F2-DB4F-8888-7076AB2E6683}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075A3A3E-129C-AE41-BC1B-0F827E590AA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Company Name</t>
   </si>
@@ -43,12 +43,6 @@
     <t>Tags</t>
   </si>
   <si>
-    <t>BU: AMEA, BUO: john@example.com, Test 1</t>
-  </si>
-  <si>
-    <t>BU: AMEA, BUO: bill@example.com, Test 2, Test 3</t>
-  </si>
-  <si>
     <t>Google</t>
   </si>
   <si>
@@ -56,6 +50,24 @@
   </si>
   <si>
     <t>BU: Legal, Test 1, Test 3</t>
+  </si>
+  <si>
+    <t>Examinetics Inc</t>
+  </si>
+  <si>
+    <t>Totally Bogus Company</t>
+  </si>
+  <si>
+    <t>BU: AMEA,VO:bill@example.com,REG:GDPR</t>
+  </si>
+  <si>
+    <t>BU: AMEA, VO: bill@example.com, Test 2, Test 3</t>
+  </si>
+  <si>
+    <t>BU: AMEA, VO: john@example.com, Test 1</t>
+  </si>
+  <si>
+    <t>BU:Legal,BU:AMEA,REG:GDPR</t>
   </si>
 </sst>
 </file>
@@ -436,7 +448,7 @@
   <dimension ref="A1:C396"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -465,7 +477,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
@@ -476,29 +488,37 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>

</xml_diff>